<commit_message>
Club visit stats in reports
</commit_message>
<xml_diff>
--- a/src/JCSGYK/AdminBundle/Resources/public/reports/homehelp_stats.xlsx
+++ b/src/JCSGYK/AdminBundle/Resources/public/reports/homehelp_stats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="1340" windowWidth="46380" windowHeight="26420"/>
@@ -132,27 +132,12 @@
     <t>Látogatások száma</t>
   </si>
   <si>
-    <t>[inv.visits;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>TM gondozottak óra / fő</t>
   </si>
   <si>
-    <t>[inv.disc;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[inv.disccli;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>Fizetős gondozottak óra / fő</t>
   </si>
   <si>
-    <t>[inv.pay;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[inv.paycli;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>Átlag gondozási órák 0.5 fő</t>
   </si>
   <si>
@@ -175,6 +160,21 @@
   </si>
   <si>
     <t>[cnum.inpatient;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[inv.disc; ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[inv.pay; ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[inv.disccli; ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[inv.visits; ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[inv.paycli; ope=tbs:num]</t>
   </si>
 </sst>
 </file>
@@ -468,23 +468,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="177">
@@ -1077,18 +1077,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
@@ -1111,127 +1111,127 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="8"/>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
       <c r="I3" s="7" t="s">
         <v>35</v>
       </c>
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
       <c r="I4" s="7" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="F5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="7" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="7" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="8"/>
-      <c r="F6" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="F6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
       <c r="I6" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
+      <c r="F7" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
       <c r="I7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="14"/>
+        <v>40</v>
+      </c>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="F8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
       <c r="I8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J8" s="14"/>
+        <v>44</v>
+      </c>
+      <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
       <c r="A9" s="2"/>
@@ -1239,42 +1239,42 @@
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="F9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
       <c r="I9" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="F10" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
       <c r="I10" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="7" t="s">
         <v>30</v>
       </c>
@@ -1286,11 +1286,11 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="7" t="s">
         <v>31</v>
       </c>
@@ -1314,10 +1314,10 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="30" customHeight="1">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="10"/>
@@ -1330,7 +1330,7 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:18" ht="21" customHeight="1">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -1346,7 +1346,7 @@
       <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:18" ht="21" customHeight="1">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -1362,10 +1362,10 @@
       <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10" ht="21" customHeight="1">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="10"/>
@@ -1378,7 +1378,7 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="21" customHeight="1">
-      <c r="A18" s="17"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="12" t="s">
         <v>21</v>
       </c>
@@ -1392,10 +1392,10 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10" ht="21" customHeight="1">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="10"/>
@@ -1408,7 +1408,7 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="21" customHeight="1">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="12" t="s">
         <v>23</v>
       </c>
@@ -1422,10 +1422,10 @@
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10" ht="21" customHeight="1">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="10"/>
@@ -1438,7 +1438,7 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="21" customHeight="1">
-      <c r="A22" s="17"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="12" t="s">
         <v>25</v>
       </c>
@@ -1561,11 +1561,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A11:C11"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="F5:H5"/>
@@ -1582,6 +1577,11 @@
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H10"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A11:C11"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.8" right="0.2" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Homehelp stat tpl fix
</commit_message>
<xml_diff>
--- a/src/JCSGYK/AdminBundle/Resources/public/reports/homehelp_stats.xlsx
+++ b/src/JCSGYK/AdminBundle/Resources/public/reports/homehelp_stats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="1340" windowWidth="46380" windowHeight="26420"/>
@@ -105,12 +105,6 @@
     <t>[inv.sum]</t>
   </si>
   <si>
-    <t>Étkezők száma NŐ</t>
-  </si>
-  <si>
-    <t>Étkezők száma FÉRFI</t>
-  </si>
-  <si>
     <t>[cnum.woman;ope=tbs:num]</t>
   </si>
   <si>
@@ -175,6 +169,12 @@
   </si>
   <si>
     <t>[inv.paycli; ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>Gondozottak száma NŐ</t>
+  </si>
+  <si>
+    <t>Gondozottak száma FÉRFI</t>
   </si>
 </sst>
 </file>
@@ -477,14 +477,14 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="177">
@@ -1077,18 +1077,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
@@ -1121,12 +1121,12 @@
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
       <c r="I3" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J3" s="8"/>
     </row>
@@ -1141,12 +1141,12 @@
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
@@ -1160,37 +1160,37 @@
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
       <c r="A6" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
@@ -1204,12 +1204,12 @@
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
       <c r="I7" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J7" s="13"/>
     </row>
@@ -1224,12 +1224,12 @@
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="I8" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J8" s="13"/>
     </row>
@@ -1240,12 +1240,12 @@
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
       <c r="F9" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
       <c r="I9" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J9" s="2"/>
     </row>
@@ -1260,23 +1260,23 @@
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
       <c r="I10" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
       <c r="A11" s="17" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1287,12 +1287,12 @@
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
       <c r="A12" s="17" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1362,7 +1362,7 @@
       <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10" ht="21" customHeight="1">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="15" t="s">
@@ -1378,7 +1378,7 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="21" customHeight="1">
-      <c r="A18" s="16"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="12" t="s">
         <v>21</v>
       </c>
@@ -1392,7 +1392,7 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10" ht="21" customHeight="1">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="18" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="15" t="s">
@@ -1408,7 +1408,7 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="21" customHeight="1">
-      <c r="A20" s="16"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="12" t="s">
         <v>23</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10" ht="21" customHeight="1">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="15" t="s">
@@ -1438,7 +1438,7 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="21" customHeight="1">
-      <c r="A22" s="16"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="12" t="s">
         <v>25</v>
       </c>
@@ -1561,6 +1561,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A11:C11"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="F5:H5"/>
@@ -1577,11 +1582,6 @@
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H10"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A11:C11"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.8" right="0.2" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>